<commit_message>
adding graphs and sketchs
</commit_message>
<xml_diff>
--- a/graphs/2neuralnetwork_graphs.xlsx
+++ b/graphs/2neuralnetwork_graphs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f398622f027937b1/Área de Trabalho/Aulas Online/Favan/TG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan\Documents\Tg\tg-preco-milho\graphs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_E0F27EC5C3F12EF5911E736F09DDE6B7502E5CA8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{AF104B18-F5EA-4579-80C0-DD888FD93FF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E4324B-1090-43DD-8C8D-4D501619CA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14252,8 +14252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E748" sqref="E748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>